<commit_message>
Update Proyecto de implantación de un ERP PLANTILLA.xlsx
</commit_message>
<xml_diff>
--- a/Gestion/Tema4/Proyecto de implantación de un ERP PLANTILLA.xlsx
+++ b/Gestion/Tema4/Proyecto de implantación de un ERP PLANTILLA.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\Portatil Medac\2DAM-Medac-Archivos\Gestion\Tema4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Portatil medac\2DAM-Medac-Archivos\Gestion\Tema4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D73C6EBA-FF8B-45BF-B09A-D590AB2A99F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83311192-28D8-48B0-85EF-499519504069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B61FB4F7-2CA4-45C6-81C7-591A9ACE023F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B61FB4F7-2CA4-45C6-81C7-591A9ACE023F}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t>Fase de la implantación</t>
   </si>
@@ -103,6 +103,66 @@
   </si>
   <si>
     <t>Se realiza un mantenimiento del ERP a largo plazo</t>
+  </si>
+  <si>
+    <t>enero,2023-febrero,2023</t>
+  </si>
+  <si>
+    <t>Si se realiza muy deprisa o de manera no adecuado todas las demas fases tendran errores</t>
+  </si>
+  <si>
+    <t>Diseño funcional</t>
+  </si>
+  <si>
+    <t>Documentacion de estimaciones del proyecto</t>
+  </si>
+  <si>
+    <t>febrero,2023-marzo,2023</t>
+  </si>
+  <si>
+    <t>Realizar esta fase incorrectamente, provocaria que errores se produjeran en las siguientes fases obligando a echar atras el proyecto para tener que volverlo a implementar</t>
+  </si>
+  <si>
+    <t>Diseño tecnico</t>
+  </si>
+  <si>
+    <t>Errores a la hora de realizar el diseño tecnico lo cual provocaria un funcionamiento inesperado</t>
+  </si>
+  <si>
+    <t>Documentacion de pruebas realizadas</t>
+  </si>
+  <si>
+    <t>marzo,2023-julio,2023</t>
+  </si>
+  <si>
+    <t>julio,2023-septiembre,2023</t>
+  </si>
+  <si>
+    <t>No descubrir errores los cuales obligaran a volver a anterior fases de implementacion cuando se descubran mas adelante</t>
+  </si>
+  <si>
+    <t>Una formacion ineficiente provocara en que los empleados puedan realizar un uso inadecuado del ERP</t>
+  </si>
+  <si>
+    <t>septiembre.2023-noviembre.2023</t>
+  </si>
+  <si>
+    <t>noviembre.2023-diciembre.2023</t>
+  </si>
+  <si>
+    <t>Un arranque mal realizado puedo llevar a que la empresa tenga que detener su funcionamiento temporalmente</t>
+  </si>
+  <si>
+    <t>diciembre,2023-enero.2023</t>
+  </si>
+  <si>
+    <t>Un mal soporte provocara que el sistema pueda tener fallos que afecten a la empresa</t>
+  </si>
+  <si>
+    <t>enero,2023-</t>
+  </si>
+  <si>
+    <t>Que cambios o actualizaciones realizadas provoquen fallos en el ERP los cuales impidan su debido funcionamiento</t>
   </si>
 </sst>
 </file>
@@ -194,7 +254,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -493,10 +553,10 @@
   <dimension ref="B2:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.28515625" customWidth="1"/>
     <col min="2" max="2" width="2.7109375" customWidth="1"/>
@@ -536,11 +596,17 @@
       <c r="D3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="H3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="2:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="1">
@@ -552,11 +618,17 @@
       <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="5" spans="2:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
@@ -568,11 +640,17 @@
       <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2" t="s">
+        <v>29</v>
+      </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="6" spans="2:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
@@ -584,11 +662,17 @@
       <c r="D6" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>31</v>
+      </c>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="7" spans="2:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
@@ -603,8 +687,12 @@
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="8" spans="2:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
@@ -619,8 +707,12 @@
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="9" spans="2:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
@@ -635,8 +727,12 @@
       <c r="E9" s="2"/>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="10" spans="2:9" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
@@ -651,8 +747,12 @@
       <c r="E10" s="2"/>
       <c r="F10" s="2"/>
       <c r="G10" s="2"/>
-      <c r="H10" s="2"/>
-      <c r="I10" s="2"/>
+      <c r="H10" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>